<commit_message>
Sửa lỗi dòng trống ở excel không hiển thị ở tệp pdf
</commit_message>
<xml_diff>
--- a/Code/ExportToPDF/Uploads/data.xlsx
+++ b/Code/ExportToPDF/Uploads/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>TT</t>
   </si>
@@ -68,13 +68,16 @@
   </si>
   <si>
     <t>Báo cáo quản lý</t>
+  </si>
+  <si>
+    <t>A1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +117,13 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -159,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -171,15 +181,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -274,6 +287,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -309,6 +339,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -487,9 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -498,20 +543,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
+      <c r="A1" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
       <c r="M1" s="2"/>
       <c r="N1" s="4" t="s">
         <v>17</v>
@@ -571,21 +618,21 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Cap nhat xuat bao cao voi kha nang tu format
</commit_message>
<xml_diff>
--- a/Code/ExportToPDF/Uploads/data.xlsx
+++ b/Code/ExportToPDF/Uploads/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>TT</t>
   </si>
@@ -68,15 +68,12 @@
   </si>
   <si>
     <t>Báo cáo quản lý</t>
-  </si>
-  <si>
-    <t>A1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,11 +185,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -287,23 +284,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -339,23 +319,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -534,7 +497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -543,22 +508,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="A1" s="8"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
       <c r="M1" s="2"/>
       <c r="N1" s="4" t="s">
         <v>17</v>

</xml_diff>